<commit_message>
Fix bug add anonymous transaction always false. Finish the excel file send for organisator
</commit_message>
<xml_diff>
--- a/public/tempFile/Summary_Fund_Collected.xlsx
+++ b/public/tempFile/Summary_Fund_Collected.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
   <si>
     <t>Summary of donation</t>
   </si>
@@ -32,13 +32,49 @@
     <t>Date of transaction</t>
   </si>
   <si>
-    <t>Michèle Collet</t>
-  </si>
-  <si>
-    <t>2020-06-09 17:53:31</t>
-  </si>
-  <si>
-    <t>2020-06-09 22:14:56</t>
+    <t>Anonymous donation</t>
+  </si>
+  <si>
+    <t>Aurore Remy</t>
+  </si>
+  <si>
+    <t>2020-06-24 13:02:24</t>
+  </si>
+  <si>
+    <t>2020-06-24 13:09:04</t>
+  </si>
+  <si>
+    <t>2020-06-24 13:11:04</t>
+  </si>
+  <si>
+    <t>2020-06-24 13:15:57</t>
+  </si>
+  <si>
+    <t>2020-06-24 13:17:22</t>
+  </si>
+  <si>
+    <t>2020-06-24 14:33:02</t>
+  </si>
+  <si>
+    <t>2020-06-24 14:34:18</t>
+  </si>
+  <si>
+    <t>2020-06-24 14:35:07</t>
+  </si>
+  <si>
+    <t>2020-06-24 14:36:57</t>
+  </si>
+  <si>
+    <t>2020-06-24 14:38:14</t>
+  </si>
+  <si>
+    <t>2020-06-24 21:14:52</t>
+  </si>
+  <si>
+    <t>2020-06-24 21:19:21</t>
+  </si>
+  <si>
+    <t>2020-06-24 21:20:00</t>
   </si>
 </sst>
 </file>
@@ -121,14 +157,14 @@
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -429,10 +465,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -443,12 +479,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -464,25 +500,155 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4">
-        <v>2000.0</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="B5" s="2">
+        <v>2268.0</v>
+      </c>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>45.0</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
         <v>12.0</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>7</v>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2">
+        <v>56.0</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2">
+        <v>123.0</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2">
+        <v>55.0</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Post search in myProject. Add filter status and translate status in column
</commit_message>
<xml_diff>
--- a/public/tempFile/Summary_Fund_Collected.xlsx
+++ b/public/tempFile/Summary_Fund_Collected.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>Summary of donation</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>2020-06-24 21:20:00</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -465,7 +468,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="C18" sqref="C18"/>
@@ -651,6 +654,14 @@
         <v>19</v>
       </c>
     </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>2634</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>